<commit_message>
Pushing Update for minor changes to wakanda/asgard
</commit_message>
<xml_diff>
--- a/Asgard_intf_selectors.xlsx
+++ b/Asgard_intf_selectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6686E0-483E-4591-9FA9-51053DF10943}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DCB9B3-9FF2-4E52-91E4-E479A353F6A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="157">
   <si>
     <t>asgard-spine101 Interface Selectors</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>trunkPort</t>
   </si>
 </sst>
 </file>
@@ -3180,7 +3183,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54:J55"/>
+      <selection activeCell="G54" sqref="G54:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4728,7 +4731,7 @@
         <v>123</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>144</v>
@@ -4768,7 +4771,7 @@
         <v>125</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>144</v>
@@ -4869,7 +4872,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+      <selection activeCell="G54" sqref="G54:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6417,7 +6420,7 @@
         <v>123</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>144</v>
@@ -6457,7 +6460,7 @@
         <v>125</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
upgraded leafs to new hardware
</commit_message>
<xml_diff>
--- a/Asgard_intf_selectors.xlsx
+++ b/Asgard_intf_selectors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\iac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\scotttyso\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DCB9B3-9FF2-4E52-91E4-E479A353F6A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462FC853-18DF-4C1A-BE6B-C184F8474966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="121">
   <si>
     <t>asgard-spine101 Interface Selectors</t>
   </si>
@@ -322,114 +322,6 @@
     <t>1/36</t>
   </si>
   <si>
-    <t>Eth1-37</t>
-  </si>
-  <si>
-    <t>1/37</t>
-  </si>
-  <si>
-    <t>Eth1-38</t>
-  </si>
-  <si>
-    <t>1/38</t>
-  </si>
-  <si>
-    <t>Eth1-39</t>
-  </si>
-  <si>
-    <t>1/39</t>
-  </si>
-  <si>
-    <t>Eth1-40</t>
-  </si>
-  <si>
-    <t>1/40</t>
-  </si>
-  <si>
-    <t>Eth1-41</t>
-  </si>
-  <si>
-    <t>1/41</t>
-  </si>
-  <si>
-    <t>Eth1-42</t>
-  </si>
-  <si>
-    <t>1/42</t>
-  </si>
-  <si>
-    <t>Eth1-43</t>
-  </si>
-  <si>
-    <t>1/43</t>
-  </si>
-  <si>
-    <t>Eth1-44</t>
-  </si>
-  <si>
-    <t>1/44</t>
-  </si>
-  <si>
-    <t>Eth1-45</t>
-  </si>
-  <si>
-    <t>1/45</t>
-  </si>
-  <si>
-    <t>Eth1-46</t>
-  </si>
-  <si>
-    <t>1/46</t>
-  </si>
-  <si>
-    <t>Eth1-47</t>
-  </si>
-  <si>
-    <t>1/47</t>
-  </si>
-  <si>
-    <t>Eth1-48</t>
-  </si>
-  <si>
-    <t>1/48</t>
-  </si>
-  <si>
-    <t>Eth1-49</t>
-  </si>
-  <si>
-    <t>1/49</t>
-  </si>
-  <si>
-    <t>Eth1-50</t>
-  </si>
-  <si>
-    <t>1/50</t>
-  </si>
-  <si>
-    <t>Eth1-51</t>
-  </si>
-  <si>
-    <t>1/51</t>
-  </si>
-  <si>
-    <t>Eth1-52</t>
-  </si>
-  <si>
-    <t>1/52</t>
-  </si>
-  <si>
-    <t>Eth1-53</t>
-  </si>
-  <si>
-    <t>1/53</t>
-  </si>
-  <si>
-    <t>Eth1-54</t>
-  </si>
-  <si>
-    <t>1/54</t>
-  </si>
-  <si>
     <t>asgard-leaf202 Interface Selectors</t>
   </si>
   <si>
@@ -478,12 +370,6 @@
     <t>lacpActive</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -505,10 +391,16 @@
     <t>infraPort</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>trunkPort</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -1919,15 +1811,15 @@
         <v>75</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="3" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1953,15 +1845,15 @@
         <v>77</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="4" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -3001,15 +2893,15 @@
         <v>75</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="3" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -3035,15 +2927,15 @@
         <v>77</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="4" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -3180,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54:G55"/>
+      <selection activeCell="G28" sqref="G28:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3970,12 +3862,20 @@
       <c r="F28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
@@ -4026,12 +3926,24 @@
       <c r="F30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
@@ -4054,12 +3966,24 @@
       <c r="F31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
@@ -4082,12 +4006,24 @@
       <c r="F32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
@@ -4110,12 +4046,24 @@
       <c r="F33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
@@ -4231,7 +4179,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -4259,7 +4207,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
@@ -4287,579 +4235,16 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1">
-        <v>201</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2">
-        <v>201</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1">
-        <v>201</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>201</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1">
-        <v>201</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2">
-        <v>201</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1">
-        <v>201</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2">
-        <v>201</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>201</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-      <c r="C49" s="2">
-        <v>201</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <v>201</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2">
-        <v>201</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1">
-        <v>201</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="2">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2">
-        <v>201</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-    </row>
-    <row r="54" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>201</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" s="2">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2">
-        <v>201</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>201</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="2">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2">
-        <v>201</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:N2"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A4:A57" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A4:A39" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"intf_selector"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H4:H51 H56:H57" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>"access,breakout,port-channel,vpc"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H52:H55" xr:uid="{7D0CD867-69D6-4FD1-9EC4-DD11B220B060}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H4:H39" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"access,breakout,port-channel,vpc"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4869,10 +4254,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54:G55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4890,7 +4275,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -4979,7 +4364,7 @@
         <v>202</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
@@ -5007,7 +4392,7 @@
         <v>202</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
@@ -5035,7 +4420,7 @@
         <v>202</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>22</v>
@@ -5063,7 +4448,7 @@
         <v>202</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -5091,7 +4476,7 @@
         <v>202</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>26</v>
@@ -5119,7 +4504,7 @@
         <v>202</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>28</v>
@@ -5147,7 +4532,7 @@
         <v>202</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>30</v>
@@ -5175,7 +4560,7 @@
         <v>202</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>32</v>
@@ -5203,7 +4588,7 @@
         <v>202</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>34</v>
@@ -5231,7 +4616,7 @@
         <v>202</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>36</v>
@@ -5259,7 +4644,7 @@
         <v>202</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>38</v>
@@ -5287,7 +4672,7 @@
         <v>202</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>40</v>
@@ -5315,7 +4700,7 @@
         <v>202</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>42</v>
@@ -5343,7 +4728,7 @@
         <v>202</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>44</v>
@@ -5371,7 +4756,7 @@
         <v>202</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>46</v>
@@ -5399,7 +4784,7 @@
         <v>202</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>48</v>
@@ -5427,7 +4812,7 @@
         <v>202</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>50</v>
@@ -5455,7 +4840,7 @@
         <v>202</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>52</v>
@@ -5483,7 +4868,7 @@
         <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>54</v>
@@ -5511,7 +4896,7 @@
         <v>202</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>56</v>
@@ -5539,7 +4924,7 @@
         <v>202</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>58</v>
@@ -5567,7 +4952,7 @@
         <v>202</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>60</v>
@@ -5595,7 +4980,7 @@
         <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>62</v>
@@ -5612,7 +4997,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -5623,7 +5008,7 @@
         <v>202</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>64</v>
@@ -5640,7 +5025,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -5651,24 +5036,32 @@
         <v>202</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="K28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -5679,7 +5072,7 @@
         <v>202</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>68</v>
@@ -5707,7 +5100,7 @@
         <v>202</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>70</v>
@@ -5715,12 +5108,24 @@
       <c r="F30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
@@ -5735,7 +5140,7 @@
         <v>202</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>72</v>
@@ -5743,12 +5148,24 @@
       <c r="F31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
@@ -5763,7 +5180,7 @@
         <v>202</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>74</v>
@@ -5771,12 +5188,24 @@
       <c r="F32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
@@ -5791,7 +5220,7 @@
         <v>202</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>76</v>
@@ -5799,12 +5228,24 @@
       <c r="F33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
@@ -5819,7 +5260,7 @@
         <v>202</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>78</v>
@@ -5847,7 +5288,7 @@
         <v>202</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>80</v>
@@ -5875,7 +5316,7 @@
         <v>202</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>82</v>
@@ -5903,7 +5344,7 @@
         <v>202</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>84</v>
@@ -5931,7 +5372,7 @@
         <v>202</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>90</v>
@@ -5948,7 +5389,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
@@ -5959,7 +5400,7 @@
         <v>202</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>92</v>
@@ -5976,582 +5417,23 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1">
-        <v>202</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2">
-        <v>202</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1">
-        <v>202</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>202</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1">
-        <v>202</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2">
-        <v>202</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1">
-        <v>202</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2">
-        <v>202</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>202</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
-      <c r="C49" s="2">
-        <v>202</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <v>202</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2">
-        <v>202</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1">
-        <v>202</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="2">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2">
-        <v>202</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-    </row>
-    <row r="54" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>202</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" s="2">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2">
-        <v>202</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>202</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="2">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2">
-        <v>202</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:N2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A57" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A39" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"intf_selector"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H50 H52:H57" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H27 H29:H39" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"access,breakout,port-channel,vpc"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H51" xr:uid="{3231675E-024D-4F4A-8AE7-A21340BCCC9F}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H28" xr:uid="{21571E1E-D800-451F-B53B-47D8932D5887}">
       <formula1>"access,breakout,port-channel,vpc"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>